<commit_message>
Auto-committed on 2022/07/22 週五 17:39:50.92
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/L1-顧客管理作業/CustMain.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/L1-顧客管理作業/CustMain.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\SKL\DB\GenTables\L1-顧客管理作業\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34C696DF-4CEA-4E56-AFD0-3B1078ABD420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2DBCBCC-EA98-4D4F-9F72-021579F60578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DBD" sheetId="1" r:id="rId1"/>
     <sheet name="DBS" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -165,30 +165,6 @@
     <t>SpouseName</t>
   </si>
   <si>
-    <t>戶籍-路名</t>
-  </si>
-  <si>
-    <t>戶籍-段</t>
-  </si>
-  <si>
-    <t>戶籍-巷</t>
-  </si>
-  <si>
-    <t>戶籍-弄</t>
-  </si>
-  <si>
-    <t>戶籍-號</t>
-  </si>
-  <si>
-    <t>戶籍-號之</t>
-  </si>
-  <si>
-    <t>戶籍-樓</t>
-  </si>
-  <si>
-    <t>戶籍-樓之</t>
-  </si>
-  <si>
     <t>通訊-郵遞區號前三碼</t>
   </si>
   <si>
@@ -698,22 +674,6 @@
   </si>
   <si>
     <t>客戶資料主檔</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>戶籍-縣市代碼</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>戶籍-鄉鎮市區代碼</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>戶籍-郵遞區號前三碼</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>戶籍-郵遞區號後三碼</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -982,6 +942,54 @@
   </si>
   <si>
     <t>是否資訊日期</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>戶籍/公司-郵遞區號前三碼</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>戶籍/公司-郵遞區號後三碼</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>戶籍/公司-縣市代碼</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>戶籍/公司-鄉鎮市區代碼</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>戶籍/公司-路名</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>戶籍/公司-段</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>戶籍/公司-巷</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>戶籍/公司-弄</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>戶籍/公司-號</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>戶籍/公司-號之</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>戶籍/公司-樓</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>戶籍/公司-樓之</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1647,8 +1655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.44140625" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -1664,14 +1672,14 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="42" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B1" s="43"/>
       <c r="C1" s="8" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="E1" s="10"/>
       <c r="F1" s="11"/>
@@ -1681,10 +1689,10 @@
       <c r="A2" s="42"/>
       <c r="B2" s="43"/>
       <c r="C2" s="12" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="14"/>
@@ -1692,14 +1700,14 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="42" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B3" s="43"/>
       <c r="C3" s="8" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="E3" s="10"/>
       <c r="F3" s="14"/>
@@ -1718,14 +1726,14 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="42" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B5" s="43"/>
       <c r="C5" s="15" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="E5" s="10"/>
       <c r="F5" s="14"/>
@@ -1733,11 +1741,11 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="42" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B6" s="43"/>
       <c r="C6" s="15" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="D6" s="16"/>
       <c r="E6" s="10"/>
@@ -1746,11 +1754,11 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="42" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B7" s="43"/>
       <c r="C7" s="15" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D7" s="16"/>
       <c r="E7" s="10"/>
@@ -1759,7 +1767,7 @@
     </row>
     <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>12</v>
@@ -1785,10 +1793,10 @@
         <v>1</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="D9" s="36" t="s">
         <v>10</v>
@@ -1805,10 +1813,10 @@
         <v>2</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="D10" s="36" t="s">
         <v>10</v>
@@ -1825,20 +1833,20 @@
         <v>3</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="D11" s="36" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="E11" s="36">
         <v>7</v>
       </c>
       <c r="F11" s="18"/>
       <c r="G11" s="18" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -1847,7 +1855,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="C12" s="18" t="s">
         <v>18</v>
@@ -1867,7 +1875,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C13" s="18" t="s">
         <v>3</v>
@@ -1893,7 +1901,7 @@
         <v>4</v>
       </c>
       <c r="D14" s="36" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="E14" s="36">
         <v>8</v>
@@ -1907,7 +1915,7 @@
         <v>7</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="C15" s="18" t="s">
         <v>5</v>
@@ -1920,7 +1928,7 @@
       </c>
       <c r="F15" s="18"/>
       <c r="G15" s="18" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="162" x14ac:dyDescent="0.3">
@@ -1929,7 +1937,7 @@
         <v>8</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C16" s="18" t="s">
         <v>6</v>
@@ -1942,7 +1950,7 @@
       </c>
       <c r="F16" s="18"/>
       <c r="G16" s="18" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="32.4" x14ac:dyDescent="0.3">
@@ -1951,7 +1959,7 @@
         <v>9</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="C17" s="18" t="s">
         <v>7</v>
@@ -1964,7 +1972,7 @@
       </c>
       <c r="F17" s="18"/>
       <c r="G17" s="18" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="32.4" x14ac:dyDescent="0.3">
@@ -1973,10 +1981,10 @@
         <v>10</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="D18" s="36" t="s">
         <v>10</v>
@@ -1986,7 +1994,7 @@
       </c>
       <c r="F18" s="18"/>
       <c r="G18" s="18" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="48.6" x14ac:dyDescent="0.3">
@@ -1995,10 +2003,10 @@
         <v>11</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="D19" s="36" t="s">
         <v>10</v>
@@ -2008,7 +2016,7 @@
       </c>
       <c r="F19" s="18"/>
       <c r="G19" s="25" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="32.4" x14ac:dyDescent="0.3">
@@ -2020,7 +2028,7 @@
         <v>21</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="D20" s="36" t="s">
         <v>10</v>
@@ -2057,10 +2065,10 @@
         <v>14</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>169</v>
+        <v>219</v>
       </c>
       <c r="D22" s="36" t="s">
         <v>10</v>
@@ -2077,10 +2085,10 @@
         <v>15</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>170</v>
+        <v>220</v>
       </c>
       <c r="D23" s="36" t="s">
         <v>10</v>
@@ -2097,10 +2105,10 @@
         <v>16</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>167</v>
+        <v>221</v>
       </c>
       <c r="D24" s="36" t="s">
         <v>10</v>
@@ -2110,7 +2118,7 @@
       </c>
       <c r="F24" s="18"/>
       <c r="G24" s="18" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -2119,10 +2127,10 @@
         <v>17</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>168</v>
+        <v>222</v>
       </c>
       <c r="D25" s="36" t="s">
         <v>10</v>
@@ -2132,7 +2140,7 @@
       </c>
       <c r="F25" s="18"/>
       <c r="G25" s="18" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -2141,10 +2149,10 @@
         <v>18</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>23</v>
+        <v>223</v>
       </c>
       <c r="D26" s="36" t="s">
         <v>19</v>
@@ -2161,10 +2169,10 @@
         <v>19</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>24</v>
+        <v>224</v>
       </c>
       <c r="D27" s="36" t="s">
         <v>10</v>
@@ -2181,10 +2189,10 @@
         <v>20</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>25</v>
+        <v>225</v>
       </c>
       <c r="D28" s="36" t="s">
         <v>10</v>
@@ -2201,10 +2209,10 @@
         <v>21</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>26</v>
+        <v>226</v>
       </c>
       <c r="D29" s="36" t="s">
         <v>10</v>
@@ -2221,10 +2229,10 @@
         <v>22</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>27</v>
+        <v>227</v>
       </c>
       <c r="D30" s="36" t="s">
         <v>10</v>
@@ -2241,10 +2249,10 @@
         <v>23</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>28</v>
+        <v>228</v>
       </c>
       <c r="D31" s="36" t="s">
         <v>10</v>
@@ -2261,10 +2269,10 @@
         <v>24</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>29</v>
+        <v>229</v>
       </c>
       <c r="D32" s="36" t="s">
         <v>10</v>
@@ -2281,10 +2289,10 @@
         <v>25</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>30</v>
+        <v>230</v>
       </c>
       <c r="D33" s="36" t="s">
         <v>10</v>
@@ -2301,10 +2309,10 @@
         <v>26</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D34" s="36" t="s">
         <v>10</v>
@@ -2321,10 +2329,10 @@
         <v>27</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="D35" s="36" t="s">
         <v>10</v>
@@ -2341,10 +2349,10 @@
         <v>28</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D36" s="36" t="s">
         <v>10</v>
@@ -2354,7 +2362,7 @@
       </c>
       <c r="F36" s="18"/>
       <c r="G36" s="18" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -2363,10 +2371,10 @@
         <v>29</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D37" s="36" t="s">
         <v>10</v>
@@ -2376,7 +2384,7 @@
       </c>
       <c r="F37" s="18"/>
       <c r="G37" s="18" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -2385,10 +2393,10 @@
         <v>30</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D38" s="36" t="s">
         <v>19</v>
@@ -2405,10 +2413,10 @@
         <v>31</v>
       </c>
       <c r="B39" s="18" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D39" s="36" t="s">
         <v>10</v>
@@ -2425,10 +2433,10 @@
         <v>32</v>
       </c>
       <c r="B40" s="18" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D40" s="36" t="s">
         <v>10</v>
@@ -2445,10 +2453,10 @@
         <v>33</v>
       </c>
       <c r="B41" s="18" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D41" s="36" t="s">
         <v>10</v>
@@ -2465,10 +2473,10 @@
         <v>34</v>
       </c>
       <c r="B42" s="18" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D42" s="36" t="s">
         <v>10</v>
@@ -2485,10 +2493,10 @@
         <v>35</v>
       </c>
       <c r="B43" s="18" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C43" s="18" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D43" s="36" t="s">
         <v>10</v>
@@ -2505,10 +2513,10 @@
         <v>36</v>
       </c>
       <c r="B44" s="18" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C44" s="18" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D44" s="36" t="s">
         <v>10</v>
@@ -2525,10 +2533,10 @@
         <v>37</v>
       </c>
       <c r="B45" s="18" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C45" s="18" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D45" s="36" t="s">
         <v>10</v>
@@ -2545,20 +2553,20 @@
         <v>38</v>
       </c>
       <c r="B46" s="25" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="C46" s="25" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="D46" s="37" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="E46" s="37">
         <v>1</v>
       </c>
       <c r="F46" s="25"/>
       <c r="G46" s="25" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="64.8" x14ac:dyDescent="0.3">
@@ -2567,10 +2575,10 @@
         <v>39</v>
       </c>
       <c r="B47" s="18" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C47" s="18" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="D47" s="36" t="s">
         <v>10</v>
@@ -2580,7 +2588,7 @@
       </c>
       <c r="F47" s="18"/>
       <c r="G47" s="18" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
     </row>
     <row r="48" spans="1:7" s="1" customFormat="1" ht="32.4" x14ac:dyDescent="0.3">
@@ -2589,7 +2597,7 @@
         <v>40</v>
       </c>
       <c r="B48" s="24" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C48" s="24" t="s">
         <v>9</v>
@@ -2602,7 +2610,7 @@
       </c>
       <c r="F48" s="24"/>
       <c r="G48" s="24" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="49" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -2611,10 +2619,10 @@
         <v>41</v>
       </c>
       <c r="B49" s="24" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="C49" s="24" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D49" s="38" t="s">
         <v>10</v>
@@ -2631,10 +2639,10 @@
         <v>42</v>
       </c>
       <c r="B50" s="24" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C50" s="24" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D50" s="38" t="s">
         <v>10</v>
@@ -2644,7 +2652,7 @@
       </c>
       <c r="F50" s="24"/>
       <c r="G50" s="24" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
     </row>
     <row r="51" spans="1:7" s="1" customFormat="1" ht="32.4" x14ac:dyDescent="0.3">
@@ -2653,10 +2661,10 @@
         <v>43</v>
       </c>
       <c r="B51" s="24" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="C51" s="24" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D51" s="38" t="s">
         <v>10</v>
@@ -2666,7 +2674,7 @@
       </c>
       <c r="F51" s="24"/>
       <c r="G51" s="24" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="52" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -2675,10 +2683,10 @@
         <v>44</v>
       </c>
       <c r="B52" s="24" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C52" s="24" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D52" s="38" t="s">
         <v>19</v>
@@ -2695,10 +2703,10 @@
         <v>45</v>
       </c>
       <c r="B53" s="24" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C53" s="24" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D53" s="38" t="s">
         <v>10</v>
@@ -2715,10 +2723,10 @@
         <v>46</v>
       </c>
       <c r="B54" s="24" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C54" s="24" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D54" s="38" t="s">
         <v>10</v>
@@ -2735,10 +2743,10 @@
         <v>47</v>
       </c>
       <c r="B55" s="24" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C55" s="24" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D55" s="38" t="s">
         <v>19</v>
@@ -2755,10 +2763,10 @@
         <v>48</v>
       </c>
       <c r="B56" s="24" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C56" s="24" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D56" s="38" t="s">
         <v>10</v>
@@ -2775,13 +2783,13 @@
         <v>49</v>
       </c>
       <c r="B57" s="24" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C57" s="24" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="D57" s="38" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E57" s="38">
         <v>9</v>
@@ -2795,10 +2803,10 @@
         <v>50</v>
       </c>
       <c r="B58" s="24" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="C58" s="24" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D58" s="38" t="s">
         <v>10</v>
@@ -2808,7 +2816,7 @@
       </c>
       <c r="F58" s="24"/>
       <c r="G58" s="24" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
     </row>
     <row r="59" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -2817,10 +2825,10 @@
         <v>51</v>
       </c>
       <c r="B59" s="24" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="C59" s="24" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D59" s="38" t="s">
         <v>10</v>
@@ -2837,10 +2845,10 @@
         <v>52</v>
       </c>
       <c r="B60" s="24" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C60" s="24" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D60" s="38" t="s">
         <v>10</v>
@@ -2857,10 +2865,10 @@
         <v>53</v>
       </c>
       <c r="B61" s="24" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C61" s="24" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D61" s="38" t="s">
         <v>10</v>
@@ -2877,10 +2885,10 @@
         <v>54</v>
       </c>
       <c r="B62" s="18" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C62" s="18" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D62" s="36" t="s">
         <v>19</v>
@@ -2897,13 +2905,13 @@
         <v>55</v>
       </c>
       <c r="B63" s="24" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="C63" s="24" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="D63" s="38" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="E63" s="38">
         <v>3</v>
@@ -2917,13 +2925,13 @@
         <v>56</v>
       </c>
       <c r="B64" s="24" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="C64" s="24" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D64" s="38" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="E64" s="38">
         <v>3</v>
@@ -2937,20 +2945,20 @@
         <v>57</v>
       </c>
       <c r="B65" s="24" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="C65" s="24" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="D65" s="38" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="E65" s="38">
         <v>1</v>
       </c>
       <c r="F65" s="24"/>
       <c r="G65" s="24" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
@@ -2959,10 +2967,10 @@
         <v>58</v>
       </c>
       <c r="B66" s="18" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="C66" s="18" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D66" s="36" t="s">
         <v>10</v>
@@ -2979,20 +2987,20 @@
         <v>59</v>
       </c>
       <c r="B67" s="19" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="C67" s="20" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="D67" s="23" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E67" s="23">
         <v>1</v>
       </c>
       <c r="F67" s="21"/>
       <c r="G67" s="22" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="32.4" x14ac:dyDescent="0.3">
@@ -3001,10 +3009,10 @@
         <v>60</v>
       </c>
       <c r="B68" s="27" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="C68" s="28" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="D68" s="37" t="s">
         <v>10</v>
@@ -3014,7 +3022,7 @@
       </c>
       <c r="F68" s="29"/>
       <c r="G68" s="28" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="32.4" x14ac:dyDescent="0.3">
@@ -3023,10 +3031,10 @@
         <v>61</v>
       </c>
       <c r="B69" s="30" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="C69" s="31" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="D69" s="39" t="s">
         <v>10</v>
@@ -3036,7 +3044,7 @@
       </c>
       <c r="F69" s="32"/>
       <c r="G69" s="31" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="48.6" x14ac:dyDescent="0.3">
@@ -3045,10 +3053,10 @@
         <v>62</v>
       </c>
       <c r="B70" s="27" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="C70" s="28" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="D70" s="37" t="s">
         <v>10</v>
@@ -3058,7 +3066,7 @@
       </c>
       <c r="F70" s="29"/>
       <c r="G70" s="28" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="48.6" x14ac:dyDescent="0.3">
@@ -3067,10 +3075,10 @@
         <v>63</v>
       </c>
       <c r="B71" s="27" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="C71" s="28" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="D71" s="37" t="s">
         <v>10</v>
@@ -3080,7 +3088,7 @@
       </c>
       <c r="F71" s="29"/>
       <c r="G71" s="28" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="48.6" x14ac:dyDescent="0.3">
@@ -3089,10 +3097,10 @@
         <v>64</v>
       </c>
       <c r="B72" s="27" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="C72" s="28" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="D72" s="37" t="s">
         <v>10</v>
@@ -3102,7 +3110,7 @@
       </c>
       <c r="F72" s="29"/>
       <c r="G72" s="28" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="32.4" x14ac:dyDescent="0.3">
@@ -3111,10 +3119,10 @@
         <v>65</v>
       </c>
       <c r="B73" s="33" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="C73" s="34" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="D73" s="40" t="s">
         <v>10</v>
@@ -3124,7 +3132,7 @@
       </c>
       <c r="F73" s="35"/>
       <c r="G73" s="34" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="32.4" x14ac:dyDescent="0.3">
@@ -3133,10 +3141,10 @@
         <v>66</v>
       </c>
       <c r="B74" s="33" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="C74" s="34" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="D74" s="40" t="s">
         <v>10</v>
@@ -3146,7 +3154,7 @@
       </c>
       <c r="F74" s="35"/>
       <c r="G74" s="34" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="32.4" x14ac:dyDescent="0.3">
@@ -3155,10 +3163,10 @@
         <v>67</v>
       </c>
       <c r="B75" s="33" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="C75" s="34" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="D75" s="40" t="s">
         <v>10</v>
@@ -3168,7 +3176,7 @@
       </c>
       <c r="F75" s="35"/>
       <c r="G75" s="34" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
@@ -3177,20 +3185,20 @@
         <v>68</v>
       </c>
       <c r="B76" s="33" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="C76" s="34" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="D76" s="40" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="E76" s="40">
         <v>8</v>
       </c>
       <c r="F76" s="35"/>
       <c r="G76" s="34" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="48.6" x14ac:dyDescent="0.3">
@@ -3199,20 +3207,20 @@
         <v>69</v>
       </c>
       <c r="B77" s="27" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="C77" s="28" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="D77" s="37" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="E77" s="37">
         <v>1</v>
       </c>
       <c r="F77" s="29"/>
       <c r="G77" s="28" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
@@ -3221,20 +3229,20 @@
         <v>70</v>
       </c>
       <c r="B78" s="27" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="C78" s="28" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="D78" s="37" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="E78" s="41">
         <v>1</v>
       </c>
       <c r="F78" s="29"/>
       <c r="G78" s="28" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="32.4" x14ac:dyDescent="0.3">
@@ -3243,10 +3251,10 @@
         <v>71</v>
       </c>
       <c r="B79" s="30" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="C79" s="31" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="D79" s="39" t="s">
         <v>10</v>
@@ -3256,7 +3264,7 @@
       </c>
       <c r="F79" s="32"/>
       <c r="G79" s="31" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
@@ -3265,13 +3273,13 @@
         <v>72</v>
       </c>
       <c r="B80" s="18" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="C80" s="18" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D80" s="36" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="E80" s="36"/>
       <c r="F80" s="18"/>
@@ -3283,10 +3291,10 @@
         <v>73</v>
       </c>
       <c r="B81" s="18" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C81" s="18" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="D81" s="36" t="s">
         <v>10</v>
@@ -3303,13 +3311,13 @@
         <v>74</v>
       </c>
       <c r="B82" s="18" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C82" s="18" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D82" s="36" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="E82" s="36"/>
       <c r="F82" s="18"/>
@@ -3320,10 +3328,10 @@
         <v>75</v>
       </c>
       <c r="B83" s="18" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C83" s="18" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D83" s="36" t="s">
         <v>10</v>
@@ -3337,7 +3345,7 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D90" s="6" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
@@ -3392,92 +3400,92 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>